<commit_message>
storage of variables 2
</commit_message>
<xml_diff>
--- a/26_AssemblyLanguage/Stack Frame.xlsx
+++ b/26_AssemblyLanguage/Stack Frame.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\Computer\C-Code\26_AssemblyLanguage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E97CD9B-AFBE-40E1-9BDD-1EBC74E4851F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88D1390-68F0-4538-904E-565C7D326048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="309" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="309" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="函数调用分析" sheetId="2" r:id="rId1"/>
@@ -219,18 +219,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1382,8 +1382,21 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>	int c = a + b;</a:t>
-          </a:r>
+            <a:t>	int c = a + b;   #</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>下面就是本行的具体寄存器操作</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -2071,7 +2084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBA8C85-79A6-4A22-9D08-55E58E08DFDF}">
   <dimension ref="B1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:H1"/>
     </sheetView>
   </sheetViews>
@@ -2081,11 +2094,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
@@ -2311,7 +2324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:I84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
@@ -2418,66 +2431,66 @@
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
-      <c r="G25" s="8"/>
+      <c r="G25" s="9"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
-      <c r="G26" s="8"/>
+      <c r="G26" s="9"/>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
-      <c r="G27" s="8"/>
+      <c r="G27" s="9"/>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G28" s="8"/>
+      <c r="G28" s="9"/>
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G29" s="8"/>
+      <c r="G29" s="9"/>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G30" s="9"/>
+      <c r="G30" s="10"/>
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G31" s="9"/>
+      <c r="G31" s="10"/>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G32" s="9"/>
+      <c r="G32" s="10"/>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="9"/>
+      <c r="G33" s="10"/>
     </row>
     <row r="61" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F61" s="3"/>
     </row>
     <row r="77" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F77" s="3"/>
-      <c r="G77" s="9"/>
+      <c r="G77" s="10"/>
       <c r="H77" s="3"/>
     </row>
     <row r="78" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="G78" s="9"/>
+      <c r="G78" s="10"/>
     </row>
     <row r="79" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="G79" s="9"/>
+      <c r="G79" s="10"/>
     </row>
     <row r="80" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="G80" s="9"/>
+      <c r="G80" s="10"/>
     </row>
     <row r="81" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F81" s="3"/>
-      <c r="G81" s="9"/>
+      <c r="G81" s="10"/>
       <c r="H81" s="3"/>
     </row>
     <row r="82" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="G82" s="9"/>
+      <c r="G82" s="10"/>
     </row>
     <row r="83" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="G83" s="9"/>
+      <c r="G83" s="10"/>
     </row>
     <row r="84" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="G84" s="9"/>
+      <c r="G84" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>